<commit_message>
Finished unit testing for Board class.
</commit_message>
<xml_diff>
--- a/docs/单元测试测试用例.xlsx
+++ b/docs/单元测试测试用例.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="118">
   <si>
     <r>
       <rPr>
@@ -654,6 +654,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Test Item 
 </t>
     </r>
@@ -768,6 +775,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Procedure 
 </t>
     </r>
@@ -908,16 +922,77 @@
     <t>使用JUnit运行单元测试</t>
   </si>
   <si>
+    <r>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；棋盘位置被设置</t>
+    </r>
+  </si>
+  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>单元测试</t>
+    <t>单元测试；路径覆盖测试</t>
   </si>
   <si>
     <t>李三木</t>
   </si>
   <si>
     <t>UT-002</t>
+  </si>
+  <si>
+    <r>
+      <t>连续两次落子；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>int columnNumber=1,int chessNumber=2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>int columnNumber=1,int chessNumber=1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；棋盘位置未被设置</t>
+    </r>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>UT-003</t>
   </si>
   <si>
     <r>
@@ -929,23 +1004,58 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>边界值测试</t>
+      <t>过小</t>
     </r>
   </si>
   <si>
     <t>int columnNumber=-1,int chessNumber=1</t>
   </si>
   <si>
-    <t>单元测试；边界值测试</t>
+    <r>
+      <t>FALSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；棋盘位置未被设置</t>
+    </r>
   </si>
   <si>
-    <t>UT-003</t>
+    <t>单元测试；条件判定白盒测试；</t>
+  </si>
+  <si>
+    <t>UT-004</t>
+  </si>
+  <si>
+    <r>
+      <t>columnNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>过大</t>
+    </r>
   </si>
   <si>
     <t>int columnNumber=7,int chessNumber=1</t>
   </si>
   <si>
-    <t>UT-004</t>
+    <t>UT-005</t>
+  </si>
+  <si>
+    <t>列满时落子</t>
+  </si>
+  <si>
+    <t>将Board置满</t>
+  </si>
+  <si>
+    <t>UT-006</t>
   </si>
   <si>
     <r>
@@ -957,26 +1067,121 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>Number边界值测试</t>
+      <t>Number类型为空棋子</t>
     </r>
+  </si>
+  <si>
+    <t>中</t>
   </si>
   <si>
     <t>int columnNumber=1,int chessNumber=0</t>
   </si>
   <si>
-    <t>NG</t>
+    <r>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；棋盘位置被设置为无效值</t>
+    </r>
   </si>
   <si>
-    <t>UT-005</t>
+    <t>单元测试；边界值测试</t>
   </si>
   <si>
-    <t>chessNumber边界值测试</t>
+    <t>UT-007</t>
+  </si>
+  <si>
+    <r>
+      <t>chessNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无效</t>
+    </r>
   </si>
   <si>
     <t>int columnNumber=1,int chessNumber=3</t>
   </si>
   <si>
     <t>单元测试；场景法测试</t>
+  </si>
+  <si>
+    <t>UT-008</t>
+  </si>
+  <si>
+    <t>sse.Board#getGameBoard</t>
+  </si>
+  <si>
+    <t>空棋盘</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <r>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>JUnit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运行单元测试</t>
+    </r>
+  </si>
+  <si>
+    <t>返回的数组与棋盘相同，且为深拷贝</t>
+  </si>
+  <si>
+    <t>返回数组内容相同，hashCode不同</t>
+  </si>
+  <si>
+    <t>单元测试；等价类测试</t>
+  </si>
+  <si>
+    <t>UT-009</t>
+  </si>
+  <si>
+    <t>棋盘有落子</t>
+  </si>
+  <si>
+    <t>在Board上落子</t>
+  </si>
+  <si>
+    <t>UT-010</t>
+  </si>
+  <si>
+    <t>满棋盘</t>
+  </si>
+  <si>
+    <t>UT-011</t>
+  </si>
+  <si>
+    <t>sse.Board#isFull</t>
+  </si>
+  <si>
+    <t>UT-012</t>
+  </si>
+  <si>
+    <t>UT-013</t>
   </si>
   <si>
     <r>
@@ -1603,13 +1808,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yy\.mm\.dd"/>
     <numFmt numFmtId="177" formatCode="yyyy\.mm\.dd"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="40">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -1713,20 +1918,49 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1740,43 +1974,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -1784,6 +1981,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1808,7 +2006,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1829,6 +2027,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1837,46 +2066,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Con"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1932,7 +2125,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1944,55 +2281,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2004,115 +2299,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2292,35 +2485,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2349,17 +2533,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2389,151 +2573,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="27" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2907,13 +3100,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-3.05177333462186e-6</c:v>
+                  <c:v>-1.01726605678176e-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.03451555641457e-6</c:v>
+                  <c:v>-3.05179817034527e-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3485,7 +3678,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="27">
         <f>65535-COUNTBLANK(单元测试!A:A)</f>
-        <v>-983035</v>
+        <v>-983027</v>
       </c>
       <c r="F11" s="28"/>
     </row>
@@ -3735,14 +3928,14 @@
       </c>
       <c r="C27" s="40">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=OK"))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D27" s="39" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="41">
         <f>IF(E11=0,0,C27/E11)</f>
-        <v>-3.05177333462186e-6</v>
+        <v>-1.01726605678176e-5</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -3767,14 +3960,14 @@
       </c>
       <c r="C29" s="40">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=NG"))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="41">
         <f>IF(E11=0,0,C29/E11)</f>
-        <v>-2.03451555641457e-6</v>
+        <v>-3.05179817034527e-6</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -3805,7 +3998,7 @@
       </c>
       <c r="C32" s="51">
         <f>E11</f>
-        <v>-983035</v>
+        <v>-983027</v>
       </c>
       <c r="D32" s="52"/>
       <c r="E32" s="53"/>
@@ -3827,10 +4020,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:EJ12389"/>
+  <dimension ref="A1:EJ12391"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6363636363636" defaultRowHeight="15.6"/>
@@ -4054,37 +4247,37 @@
       <c r="I2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="14" t="b">
-        <v>1</v>
+      <c r="J2" s="14" t="s">
+        <v>62</v>
       </c>
-      <c r="K2" s="14" t="b">
-        <v>1</v>
+      <c r="K2" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" ht="28.8" spans="1:16">
+    </row>
+    <row r="3" ht="72" spans="1:16">
       <c r="A3" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>66</v>
+      <c r="C3" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>57</v>
@@ -4098,43 +4291,43 @@
       <c r="G3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>67</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="14" t="b">
-        <v>0</v>
+      <c r="J3" s="14" t="s">
+        <v>62</v>
       </c>
-      <c r="K3" s="14" t="b">
-        <v>0</v>
+      <c r="K3" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="28.8" spans="1:16">
       <c r="A4" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>57</v>
@@ -4149,42 +4342,42 @@
         <v>59</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="14" t="b">
-        <v>0</v>
+      <c r="J4" s="14" t="s">
+        <v>73</v>
       </c>
-      <c r="K4" s="14" t="b">
-        <v>0</v>
+      <c r="K4" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:16">
       <c r="A5" s="14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>57</v>
@@ -4199,42 +4392,42 @@
         <v>59</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="14" t="b">
-        <v>0</v>
+      <c r="J5" s="14" t="s">
+        <v>73</v>
       </c>
-      <c r="K5" s="14" t="b">
-        <v>1</v>
+      <c r="K5" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="L5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="N5" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" ht="28.8" spans="1:16">
       <c r="A6" s="14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>76</v>
+      <c r="C6" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>57</v>
@@ -4246,179 +4439,435 @@
         <v>58</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="14" t="b">
+      <c r="J6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" ht="43.2" spans="1:16">
+      <c r="A7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" ht="43.2" spans="1:16">
+      <c r="A8" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" ht="43.2" spans="1:16">
+      <c r="A9" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" ht="43.2" spans="1:16">
+      <c r="A10" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" ht="43.2" spans="1:16">
+      <c r="A11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="14" t="b">
+      <c r="K12" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J14" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>74</v>
+      <c r="K14" s="14" t="b">
+        <v>1</v>
       </c>
-      <c r="M6" s="16" t="s">
-        <v>78</v>
+      <c r="L14" s="14" t="s">
+        <v>63</v>
       </c>
-      <c r="N6" s="16" t="s">
-        <v>64</v>
+      <c r="M14" s="16" t="s">
+        <v>98</v>
       </c>
-      <c r="O6" s="16" t="s">
-        <v>64</v>
+      <c r="N14" s="16" t="s">
+        <v>65</v>
       </c>
-      <c r="P6" s="16" t="s">
-        <v>62</v>
+      <c r="O14" s="16" t="s">
+        <v>65</v>
       </c>
-    </row>
-    <row r="7" ht="15" spans="1:16">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-    </row>
-    <row r="8" ht="15" spans="1:16">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-    </row>
-    <row r="9" ht="15" spans="1:16">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-    </row>
-    <row r="10" ht="15" spans="1:16">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="11" ht="15" spans="1:16">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-    </row>
-    <row r="12" ht="15" spans="1:16">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-    </row>
-    <row r="13" ht="15" spans="1:16">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" ht="15" spans="1:16">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="P14" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" ht="15" spans="1:16">
       <c r="A15" s="14"/>
@@ -5356,13 +5805,41 @@
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
     </row>
-    <row r="67" spans="12:13">
+    <row r="67" ht="15" spans="1:16">
+      <c r="A67" s="14"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
       <c r="L67" s="14"/>
       <c r="M67" s="14"/>
-    </row>
-    <row r="68" spans="12:13">
+      <c r="N67" s="14"/>
+      <c r="O67" s="14"/>
+      <c r="P67" s="14"/>
+    </row>
+    <row r="68" ht="15" spans="1:16">
+      <c r="A68" s="14"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
       <c r="L68" s="14"/>
       <c r="M68" s="14"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="14"/>
+      <c r="P68" s="14"/>
     </row>
     <row r="69" spans="12:13">
       <c r="L69" s="14"/>
@@ -54648,14 +55125,21 @@
       <c r="L12389" s="14"/>
       <c r="M12389" s="14"/>
     </row>
+    <row r="12390" spans="12:13">
+      <c r="L12390" s="14"/>
+      <c r="M12390" s="14"/>
+    </row>
+    <row r="12391" spans="12:13">
+      <c r="L12391" s="14"/>
+      <c r="M12391" s="14"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
-  <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Invalide Data" sqref="K2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 L3:L4 L5:L6 M2:M6 L7:M12389">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 M4 L5:L6 L7:L8 L9:L10 L11:L12 L13:L14 M5:M6 M7:M8 M9:M14 L15:M12391">
       <formula1>Result</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12390:M65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12392:M65538">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -54683,7 +55167,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -54693,7 +55177,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -54702,7 +55186,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -54711,7 +55195,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -54720,7 +55204,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -54729,7 +55213,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -54738,7 +55222,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -54747,7 +55231,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -54756,7 +55240,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -54765,7 +55249,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some tests for GameController.
</commit_message>
<xml_diff>
--- a/docs/单元测试测试用例.xlsx
+++ b/docs/单元测试测试用例.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="136">
   <si>
     <r>
       <rPr>
@@ -923,6 +923,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>TRUE</t>
     </r>
     <r>
@@ -948,6 +953,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>连续两次落子；</t>
     </r>
     <r>
@@ -977,6 +987,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>TRUE</t>
     </r>
     <r>
@@ -996,6 +1011,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>columnNumber</t>
     </r>
     <r>
@@ -1012,6 +1032,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>FALSE</t>
     </r>
     <r>
@@ -1031,6 +1056,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>columnNumber</t>
     </r>
     <r>
@@ -1059,6 +1089,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>chess</t>
     </r>
     <r>
@@ -1078,6 +1113,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>TRUE</t>
     </r>
     <r>
@@ -1097,6 +1137,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>chessNumber</t>
     </r>
     <r>
@@ -1128,6 +1173,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>使用</t>
     </r>
     <r>
@@ -1182,6 +1232,96 @@
   </si>
   <si>
     <t>UT-013</t>
+  </si>
+  <si>
+    <t>UT-014</t>
+  </si>
+  <si>
+    <t>sse.GameController#setChess</t>
+  </si>
+  <si>
+    <t>正常放置棋子</t>
+  </si>
+  <si>
+    <t>新的GameController对象</t>
+  </si>
+  <si>
+    <t>int column=3</t>
+  </si>
+  <si>
+    <t>返回True，棋盘被设置，player更新</t>
+  </si>
+  <si>
+    <t>UT-015</t>
+  </si>
+  <si>
+    <t>以Player2放置棋子</t>
+  </si>
+  <si>
+    <t>当前为Player2下棋</t>
+  </si>
+  <si>
+    <r>
+      <t>Player1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>先落一子；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>int column=3</t>
+    </r>
+  </si>
+  <si>
+    <t>单元测试；判定覆盖测试</t>
+  </si>
+  <si>
+    <t>UT-016</t>
+  </si>
+  <si>
+    <t>在无效位置放置棋子</t>
+  </si>
+  <si>
+    <t>int column=7</t>
+  </si>
+  <si>
+    <t>返回False，棋盘未设置，player不变</t>
+  </si>
+  <si>
+    <t>返回False，棋盘未设置，player被切换</t>
+  </si>
+  <si>
+    <t>UT-017</t>
+  </si>
+  <si>
+    <r>
+      <t>将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>GameController</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的Board填满</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1807,12 +1947,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yy\.mm\.dd"/>
     <numFmt numFmtId="177" formatCode="yyyy\.mm\.dd"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1923,7 +2063,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1944,11 +2084,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1960,22 +2100,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1984,51 +2109,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2051,8 +2131,54 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2061,6 +2187,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2125,7 +2265,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2137,7 +2385,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2149,19 +2403,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2173,19 +2427,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2197,115 +2445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2485,11 +2625,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2518,17 +2664,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2550,11 +2692,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2577,8 +2717,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2588,10 +2728,10 @@
     <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2600,40 +2740,40 @@
     <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2642,91 +2782,91 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3100,13 +3240,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1.01726605678176e-5</c:v>
+                  <c:v>-1.22072423534343e-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.05179817034527e-6</c:v>
+                  <c:v>-5.08635098059761e-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3678,7 +3818,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="27">
         <f>65535-COUNTBLANK(单元测试!A:A)</f>
-        <v>-983027</v>
+        <v>-983023</v>
       </c>
       <c r="F11" s="28"/>
     </row>
@@ -3928,14 +4068,14 @@
       </c>
       <c r="C27" s="40">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=OK"))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D27" s="39" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="41">
         <f>IF(E11=0,0,C27/E11)</f>
-        <v>-1.01726605678176e-5</v>
+        <v>-1.22072423534343e-5</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -3960,14 +4100,14 @@
       </c>
       <c r="C29" s="40">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=NG"))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="41">
         <f>IF(E11=0,0,C29/E11)</f>
-        <v>-3.05179817034527e-6</v>
+        <v>-5.08635098059761e-6</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -3998,7 +4138,7 @@
       </c>
       <c r="C32" s="51">
         <f>E11</f>
-        <v>-983027</v>
+        <v>-983023</v>
       </c>
       <c r="D32" s="52"/>
       <c r="E32" s="53"/>
@@ -4020,10 +4160,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:EJ12391"/>
+  <dimension ref="A1:EJ12392"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13:L14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6363636363636" defaultRowHeight="15.6"/>
@@ -4719,7 +4859,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" ht="15" spans="1:16">
       <c r="A12" s="14" t="s">
         <v>104</v>
       </c>
@@ -4769,7 +4909,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" ht="15" spans="1:16">
       <c r="A13" s="14" t="s">
         <v>106</v>
       </c>
@@ -4869,77 +5009,205 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" ht="15" spans="1:16">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-    </row>
-    <row r="16" ht="15" spans="1:16">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-    </row>
-    <row r="17" ht="15" spans="1:16">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-    </row>
-    <row r="18" ht="15" spans="1:16">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
+    <row r="15" ht="43.2" spans="1:16">
+      <c r="A15" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" ht="43.2" spans="1:16">
+      <c r="A16" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" ht="43.2" spans="1:16">
+      <c r="A17" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" ht="43.2" spans="1:16">
+      <c r="A18" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" ht="15" spans="1:16">
       <c r="A19" s="14"/>
@@ -5841,9 +6109,23 @@
       <c r="O68" s="14"/>
       <c r="P68" s="14"/>
     </row>
-    <row r="69" spans="12:13">
+    <row r="69" ht="15" spans="1:16">
+      <c r="A69" s="14"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
       <c r="L69" s="14"/>
       <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="14"/>
     </row>
     <row r="70" spans="12:13">
       <c r="L70" s="14"/>
@@ -55133,13 +55415,17 @@
       <c r="L12391" s="14"/>
       <c r="M12391" s="14"/>
     </row>
+    <row r="12392" spans="12:13">
+      <c r="L12392" s="14"/>
+      <c r="M12392" s="14"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 M4 L5:L6 L7:L8 L9:L10 L11:L12 L13:L14 M5:M6 M7:M8 M9:M14 L15:M12391">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 M4 L13 M15 M16 L17 M17 L18 M18 L5:L6 L7:L8 L9:L10 L11:L12 L14:L16 M5:M6 M7:M8 M9:M14 L19:M12392">
       <formula1>Result</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12392:M65538">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12393:M65539">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -55167,7 +55453,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -55177,7 +55463,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -55186,7 +55472,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -55195,7 +55481,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -55204,7 +55490,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -55213,7 +55499,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -55222,7 +55508,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -55231,7 +55517,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -55240,7 +55526,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -55249,7 +55535,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started path test analyze on GameController#checkWinning
</commit_message>
<xml_diff>
--- a/docs/单元测试测试用例.xlsx
+++ b/docs/单元测试测试用例.xlsx
@@ -943,7 +943,7 @@
     <t>OK</t>
   </si>
   <si>
-    <t>单元测试；路径覆盖测试</t>
+    <t>单元测试；判定覆盖测试</t>
   </si>
   <si>
     <t>李三木</t>
@@ -1049,7 +1049,7 @@
     </r>
   </si>
   <si>
-    <t>单元测试；条件判定白盒测试；</t>
+    <t>单元测试；条件/判定覆盖测试；</t>
   </si>
   <si>
     <t>UT-004</t>
@@ -1262,6 +1262,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
       <t>Player1</t>
     </r>
     <r>
@@ -1282,7 +1287,7 @@
     </r>
   </si>
   <si>
-    <t>单元测试；判定覆盖测试</t>
+    <t>单元测试；条件覆盖测试</t>
   </si>
   <si>
     <t>UT-016</t>
@@ -1304,6 +1309,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>将</t>
     </r>
     <r>
@@ -1949,10 +1959,10 @@
   <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yy\.mm\.dd"/>
     <numFmt numFmtId="177" formatCode="yyyy\.mm\.dd"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -2058,7 +2068,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2071,6 +2081,59 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2085,7 +2148,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -2093,14 +2164,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2115,31 +2187,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2155,45 +2204,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2265,7 +2275,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2277,91 +2305,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2379,13 +2323,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2403,6 +2347,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2415,7 +2407,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2427,13 +2419,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2445,7 +2455,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2626,6 +2636,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2640,17 +2665,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2666,11 +2685,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2692,181 +2724,159 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="30" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4959,7 +4969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" ht="15" spans="1:16">
       <c r="A14" s="14" t="s">
         <v>107</v>
       </c>
@@ -55422,7 +55432,7 @@
   </sheetData>
   <sheetProtection formatCells="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 M4 L13 M15 M16 L17 M17 L18 M18 L5:L6 L7:L8 L9:L10 L11:L12 L14:L16 M5:M6 M7:M8 M9:M14 L19:M12392">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 L13 M15 M16 L17 M17 L18 M18 L5:L6 L7:L8 L9:L10 L11:L12 L14:L16 M4:M6 M7:M8 M9:M14 L19:M12392">
       <formula1>Result</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12393:M65539">

</xml_diff>

<commit_message>
Finished unit testing on the project.
</commit_message>
<xml_diff>
--- a/docs/单元测试测试用例.xlsx
+++ b/docs/单元测试测试用例.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="170">
   <si>
     <r>
       <rPr>
@@ -1252,6 +1252,9 @@
     <t>返回True，棋盘被设置，player更新</t>
   </si>
   <si>
+    <t>李澳</t>
+  </si>
+  <si>
     <t>UT-015</t>
   </si>
   <si>
@@ -1293,21 +1296,6 @@
     <t>UT-016</t>
   </si>
   <si>
-    <t>在无效位置放置棋子</t>
-  </si>
-  <si>
-    <t>int column=7</t>
-  </si>
-  <si>
-    <t>返回False，棋盘未设置，player不变</t>
-  </si>
-  <si>
-    <t>返回False，棋盘未设置，player被切换</t>
-  </si>
-  <si>
-    <t>UT-017</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1332,6 +1320,180 @@
       </rPr>
       <t>的Board填满</t>
     </r>
+  </si>
+  <si>
+    <t>返回False，棋盘未设置，player不变</t>
+  </si>
+  <si>
+    <t>返回False，棋盘未设置，player被切换</t>
+  </si>
+  <si>
+    <t>UT-017</t>
+  </si>
+  <si>
+    <t>column数值过小</t>
+  </si>
+  <si>
+    <t>int column=-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>JUnit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运行单元测试</t>
+    </r>
+  </si>
+  <si>
+    <t>FALSE；棋盘位置未被设置</t>
+  </si>
+  <si>
+    <t>单元测试；条件判定白盒测试；边界值测试</t>
+  </si>
+  <si>
+    <t>UT-018</t>
+  </si>
+  <si>
+    <t>column数值过大</t>
+  </si>
+  <si>
+    <t>int column=7</t>
+  </si>
+  <si>
+    <t>UT-019</t>
+  </si>
+  <si>
+    <t>sse.GameController#checkWinning</t>
+  </si>
+  <si>
+    <t>水平连续</t>
+  </si>
+  <si>
+    <t>在Board上放置水平连续的棋子</t>
+  </si>
+  <si>
+    <t>单元测试；路径覆盖测试</t>
+  </si>
+  <si>
+    <t>UT-020</t>
+  </si>
+  <si>
+    <t>垂直连续</t>
+  </si>
+  <si>
+    <r>
+      <t>在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Board</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>上放置垂直连续的棋子</t>
+    </r>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>UT-021</t>
+  </si>
+  <si>
+    <t>左上到右下对角连续</t>
+  </si>
+  <si>
+    <t>落子位置row&gt;=3;使棋子从左上到右下连续</t>
+  </si>
+  <si>
+    <t>UT-022</t>
+  </si>
+  <si>
+    <t>右上到左下对角连续</t>
+  </si>
+  <si>
+    <t>落子位置row&lt;3;使棋子从右上到左下连续</t>
+  </si>
+  <si>
+    <t>UT-023</t>
+  </si>
+  <si>
+    <t>不连续</t>
+  </si>
+  <si>
+    <t>落子位置row&lt;3;棋子在任何方向不连续</t>
+  </si>
+  <si>
+    <t>UT-024</t>
+  </si>
+  <si>
+    <t>对空棋盘调用该函数</t>
+  </si>
+  <si>
+    <t>sse.GameController#isFinished</t>
+  </si>
+  <si>
+    <t>一方获胜</t>
+  </si>
+  <si>
+    <r>
+      <t>设置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Board</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使一方获胜</t>
+    </r>
+  </si>
+  <si>
+    <t>调用该函数</t>
+  </si>
+  <si>
+    <t>棋盘满</t>
+  </si>
+  <si>
+    <t>设置棋盘满且未获胜</t>
+  </si>
+  <si>
+    <t>双方均未获胜且棋盘未满</t>
   </si>
   <si>
     <r>
@@ -1957,14 +2119,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yy\.mm\.dd"/>
-    <numFmt numFmtId="177" formatCode="yyyy\.mm\.dd"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy\.mm\.dd"/>
+    <numFmt numFmtId="177" formatCode="yy\.mm\.dd"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="45">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -2020,9 +2182,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -2068,19 +2245,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2094,7 +2279,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2102,69 +2302,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2187,8 +2324,55 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2209,18 +2393,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Con"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2275,7 +2463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2293,6 +2481,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2305,7 +2517,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2317,25 +2601,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2347,43 +2619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2395,67 +2631,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2635,6 +2823,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2646,6 +2852,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2676,54 +2912,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2735,152 +2923,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2927,14 +3115,26 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2946,7 +3146,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2958,21 +3158,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
@@ -2980,7 +3180,7 @@
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
@@ -2993,7 +3193,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3006,15 +3206,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="19" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3250,13 +3450,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1.22072423534343e-5</c:v>
+                  <c:v>-1.93282713607917e-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.08635098059761e-6</c:v>
+                  <c:v>-8.13821952033334e-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3666,492 +3866,492 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6363636363636" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="1.63636363636364" style="19" customWidth="1"/>
-    <col min="2" max="13" width="10.6363636363636" style="19" customWidth="1"/>
-    <col min="14" max="15" width="7.63636363636364" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="11.6363636363636" style="19"/>
+    <col min="1" max="1" width="1.63636363636364" style="22" customWidth="1"/>
+    <col min="2" max="13" width="10.6363636363636" style="22" customWidth="1"/>
+    <col min="14" max="15" width="7.63636363636364" style="22" customWidth="1"/>
+    <col min="16" max="16384" width="11.6363636363636" style="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="9.9" customHeight="1"/>
     <row r="2" ht="22.8" spans="2:11">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
     </row>
     <row r="3" ht="3.9" customHeight="1"/>
     <row r="4" spans="2:12">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="25" t="s">
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="23" t="s">
+      <c r="F6" s="28"/>
+      <c r="G6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="25" t="s">
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="31"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="25" t="s">
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="28"/>
+      <c r="G8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="25" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="31"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="25" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="23" t="s">
+      <c r="F9" s="28"/>
+      <c r="G9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="25" t="s">
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" ht="3.9" customHeight="1" spans="2:11">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="27">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="30">
         <f>65535-COUNTBLANK(单元测试!A:A)</f>
-        <v>-983023</v>
+        <v>-983016</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" ht="3.9" customHeight="1" spans="2:5">
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="28"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="31"/>
     </row>
     <row r="14" ht="18.9" customHeight="1" spans="2:12">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="28"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="31"/>
     </row>
     <row r="15" ht="3.9" customHeight="1" spans="2:11">
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="28"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="31"/>
     </row>
     <row r="17" ht="46.8" spans="2:12">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="31" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="28"/>
+      <c r="L17" s="31"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25" t="s">
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="28"/>
+      <c r="L18" s="31"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="37">
         <v>1.01</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25" t="s">
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="28"/>
+      <c r="L19" s="31"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="25" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25" t="s">
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="28"/>
+      <c r="L20" s="31"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="37">
         <v>1.02</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25" t="s">
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="28"/>
+      <c r="L21" s="31"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25" t="s">
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="31"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="37">
         <v>2</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25" t="s">
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="L23" s="28"/>
+      <c r="L23" s="31"/>
     </row>
     <row r="24" ht="3.9" customHeight="1" spans="2:11">
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="26" ht="15" customHeight="1" spans="2:5">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="43">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=OK"))</f>
-        <v>12</v>
+        <v>19</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="44">
         <f>IF(E11=0,0,C27/E11)</f>
-        <v>-1.22072423534343e-5</v>
+        <v>-1.93282713607917e-5</v>
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="43">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=POK"))</f>
         <v>0</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="44">
         <f>IF(E11=0,0,C28/E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="43">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=NG"))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="44">
         <f>IF(E11=0,0,C29/E11)</f>
-        <v>-5.08635098059761e-6</v>
+        <v>-8.13821952033334e-6</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="44">
+      <c r="C30" s="47">
         <f>IF($E$11=0,0,COUNTIF(单元测试!$L:$L,"=NT"))</f>
         <v>0</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="45">
+      <c r="E30" s="48">
         <f>IF(E11=0,0,C30/E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" ht="3" customHeight="1" spans="2:5">
-      <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="51">
+      <c r="C32" s="54">
         <f>E11</f>
-        <v>-983023</v>
+        <v>-983016</v>
       </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="53"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4170,10 +4370,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:EJ12392"/>
+  <dimension ref="A1:EJ12389"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6363636363636" defaultRowHeight="15.6"/>
@@ -4235,139 +4435,139 @@
       <c r="M1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
-      <c r="BG1" s="18"/>
-      <c r="BH1" s="18"/>
-      <c r="BI1" s="18"/>
-      <c r="BJ1" s="18"/>
-      <c r="BK1" s="18"/>
-      <c r="BL1" s="18"/>
-      <c r="BM1" s="18"/>
-      <c r="BN1" s="18"/>
-      <c r="BO1" s="18"/>
-      <c r="BP1" s="18"/>
-      <c r="BQ1" s="18"/>
-      <c r="BR1" s="18"/>
-      <c r="BS1" s="18"/>
-      <c r="BT1" s="18"/>
-      <c r="BU1" s="18"/>
-      <c r="BV1" s="18"/>
-      <c r="BW1" s="18"/>
-      <c r="BX1" s="18"/>
-      <c r="BY1" s="18"/>
-      <c r="BZ1" s="18"/>
-      <c r="CA1" s="18"/>
-      <c r="CB1" s="18"/>
-      <c r="CC1" s="18"/>
-      <c r="CD1" s="18"/>
-      <c r="CE1" s="18"/>
-      <c r="CF1" s="18"/>
-      <c r="CG1" s="18"/>
-      <c r="CH1" s="18"/>
-      <c r="CI1" s="18"/>
-      <c r="CJ1" s="18"/>
-      <c r="CK1" s="18"/>
-      <c r="CL1" s="18"/>
-      <c r="CM1" s="18"/>
-      <c r="CN1" s="18"/>
-      <c r="CO1" s="18"/>
-      <c r="CP1" s="18"/>
-      <c r="CQ1" s="18"/>
-      <c r="CR1" s="18"/>
-      <c r="CS1" s="18"/>
-      <c r="CT1" s="18"/>
-      <c r="CU1" s="18"/>
-      <c r="CV1" s="18"/>
-      <c r="CW1" s="18"/>
-      <c r="CX1" s="18"/>
-      <c r="CY1" s="18"/>
-      <c r="CZ1" s="18"/>
-      <c r="DA1" s="18"/>
-      <c r="DB1" s="18"/>
-      <c r="DC1" s="18"/>
-      <c r="DD1" s="18"/>
-      <c r="DE1" s="18"/>
-      <c r="DF1" s="18"/>
-      <c r="DG1" s="18"/>
-      <c r="DH1" s="18"/>
-      <c r="DI1" s="18"/>
-      <c r="DJ1" s="18"/>
-      <c r="DK1" s="18"/>
-      <c r="DL1" s="18"/>
-      <c r="DM1" s="18"/>
-      <c r="DN1" s="18"/>
-      <c r="DO1" s="18"/>
-      <c r="DP1" s="18"/>
-      <c r="DQ1" s="18"/>
-      <c r="DR1" s="18"/>
-      <c r="DS1" s="18"/>
-      <c r="DT1" s="18"/>
-      <c r="DU1" s="18"/>
-      <c r="DV1" s="18"/>
-      <c r="DW1" s="18"/>
-      <c r="DX1" s="18"/>
-      <c r="DY1" s="18"/>
-      <c r="DZ1" s="18"/>
-      <c r="EA1" s="18"/>
-      <c r="EB1" s="18"/>
-      <c r="EC1" s="18"/>
-      <c r="ED1" s="18"/>
-      <c r="EE1" s="18"/>
-      <c r="EF1" s="18"/>
-      <c r="EG1" s="18"/>
-      <c r="EH1" s="18"/>
-      <c r="EI1" s="18"/>
-      <c r="EJ1" s="18"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="21"/>
+      <c r="AK1" s="21"/>
+      <c r="AL1" s="21"/>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="21"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="21"/>
+      <c r="AT1" s="21"/>
+      <c r="AU1" s="21"/>
+      <c r="AV1" s="21"/>
+      <c r="AW1" s="21"/>
+      <c r="AX1" s="21"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="21"/>
+      <c r="BB1" s="21"/>
+      <c r="BC1" s="21"/>
+      <c r="BD1" s="21"/>
+      <c r="BE1" s="21"/>
+      <c r="BF1" s="21"/>
+      <c r="BG1" s="21"/>
+      <c r="BH1" s="21"/>
+      <c r="BI1" s="21"/>
+      <c r="BJ1" s="21"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
+      <c r="BM1" s="21"/>
+      <c r="BN1" s="21"/>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
+      <c r="BQ1" s="21"/>
+      <c r="BR1" s="21"/>
+      <c r="BS1" s="21"/>
+      <c r="BT1" s="21"/>
+      <c r="BU1" s="21"/>
+      <c r="BV1" s="21"/>
+      <c r="BW1" s="21"/>
+      <c r="BX1" s="21"/>
+      <c r="BY1" s="21"/>
+      <c r="BZ1" s="21"/>
+      <c r="CA1" s="21"/>
+      <c r="CB1" s="21"/>
+      <c r="CC1" s="21"/>
+      <c r="CD1" s="21"/>
+      <c r="CE1" s="21"/>
+      <c r="CF1" s="21"/>
+      <c r="CG1" s="21"/>
+      <c r="CH1" s="21"/>
+      <c r="CI1" s="21"/>
+      <c r="CJ1" s="21"/>
+      <c r="CK1" s="21"/>
+      <c r="CL1" s="21"/>
+      <c r="CM1" s="21"/>
+      <c r="CN1" s="21"/>
+      <c r="CO1" s="21"/>
+      <c r="CP1" s="21"/>
+      <c r="CQ1" s="21"/>
+      <c r="CR1" s="21"/>
+      <c r="CS1" s="21"/>
+      <c r="CT1" s="21"/>
+      <c r="CU1" s="21"/>
+      <c r="CV1" s="21"/>
+      <c r="CW1" s="21"/>
+      <c r="CX1" s="21"/>
+      <c r="CY1" s="21"/>
+      <c r="CZ1" s="21"/>
+      <c r="DA1" s="21"/>
+      <c r="DB1" s="21"/>
+      <c r="DC1" s="21"/>
+      <c r="DD1" s="21"/>
+      <c r="DE1" s="21"/>
+      <c r="DF1" s="21"/>
+      <c r="DG1" s="21"/>
+      <c r="DH1" s="21"/>
+      <c r="DI1" s="21"/>
+      <c r="DJ1" s="21"/>
+      <c r="DK1" s="21"/>
+      <c r="DL1" s="21"/>
+      <c r="DM1" s="21"/>
+      <c r="DN1" s="21"/>
+      <c r="DO1" s="21"/>
+      <c r="DP1" s="21"/>
+      <c r="DQ1" s="21"/>
+      <c r="DR1" s="21"/>
+      <c r="DS1" s="21"/>
+      <c r="DT1" s="21"/>
+      <c r="DU1" s="21"/>
+      <c r="DV1" s="21"/>
+      <c r="DW1" s="21"/>
+      <c r="DX1" s="21"/>
+      <c r="DY1" s="21"/>
+      <c r="DZ1" s="21"/>
+      <c r="EA1" s="21"/>
+      <c r="EB1" s="21"/>
+      <c r="EC1" s="21"/>
+      <c r="ED1" s="21"/>
+      <c r="EE1" s="21"/>
+      <c r="EF1" s="21"/>
+      <c r="EG1" s="21"/>
+      <c r="EH1" s="21"/>
+      <c r="EI1" s="21"/>
+      <c r="EJ1" s="21"/>
     </row>
     <row r="2" ht="28.8" spans="1:16">
       <c r="A2" s="14" t="s">
@@ -5059,11 +5259,11 @@
       <c r="M15" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="N15" s="16" t="s">
-        <v>65</v>
+      <c r="N15" s="18" t="s">
+        <v>114</v>
       </c>
-      <c r="O15" s="16" t="s">
-        <v>65</v>
+      <c r="O15" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="P15" s="16" t="s">
         <v>63</v>
@@ -5071,13 +5271,13 @@
     </row>
     <row r="16" ht="43.2" spans="1:16">
       <c r="A16" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>109</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>57</v>
@@ -5089,10 +5289,10 @@
         <v>58</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>61</v>
@@ -5107,13 +5307,13 @@
         <v>63</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
-      <c r="N16" s="16" t="s">
-        <v>65</v>
+      <c r="N16" s="18" t="s">
+        <v>114</v>
       </c>
-      <c r="O16" s="16" t="s">
-        <v>65</v>
+      <c r="O16" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="P16" s="16" t="s">
         <v>63</v>
@@ -5121,13 +5321,13 @@
     </row>
     <row r="17" ht="43.2" spans="1:16">
       <c r="A17" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>109</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>57</v>
@@ -5138,11 +5338,11 @@
       <c r="F17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>111</v>
+      <c r="G17" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>61</v>
@@ -5159,25 +5359,25 @@
       <c r="M17" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N17" s="16" t="s">
-        <v>65</v>
+      <c r="N17" s="18" t="s">
+        <v>114</v>
       </c>
-      <c r="O17" s="16" t="s">
-        <v>65</v>
+      <c r="O17" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="P17" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" ht="43.2" spans="1:16">
+    <row r="18" customFormat="1" ht="43.2" spans="1:16">
       <c r="A18" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>103</v>
+      <c r="C18" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>57</v>
@@ -5189,16 +5389,16 @@
         <v>58</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>112</v>
+      <c r="H18" s="17" t="s">
+        <v>126</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>61</v>
+      <c r="I18" s="16" t="s">
+        <v>127</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>122</v>
+      <c r="J18" s="20" t="s">
+        <v>128</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>123</v>
@@ -5206,200 +5406,514 @@
       <c r="L18" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="16" t="s">
-        <v>86</v>
+      <c r="M18" s="20" t="s">
+        <v>129</v>
       </c>
-      <c r="N18" s="16" t="s">
-        <v>65</v>
+      <c r="N18" s="18" t="s">
+        <v>114</v>
       </c>
-      <c r="O18" s="16" t="s">
-        <v>65</v>
+      <c r="O18" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="P18" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" ht="15" spans="1:16">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-    </row>
-    <row r="20" ht="15" spans="1:16">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-    </row>
-    <row r="21" ht="15" spans="1:16">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-    </row>
-    <row r="22" ht="15" spans="1:16">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-    </row>
-    <row r="23" ht="15" spans="1:16">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-    </row>
-    <row r="24" ht="15" spans="1:16">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-    </row>
-    <row r="25" ht="15" spans="1:16">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-    </row>
-    <row r="26" ht="15" spans="1:16">
+    <row r="19" customFormat="1" ht="43.2" spans="1:16">
+      <c r="A19" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" ht="28.8" spans="1:16">
+      <c r="A20" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" ht="28.8" spans="1:16">
+      <c r="A21" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" ht="28.8" spans="1:16">
+      <c r="A22" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J22" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" ht="28.8" spans="1:16">
+      <c r="A23" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" ht="28.8" spans="1:16">
+      <c r="A24" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O24" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" ht="28.8" spans="1:16">
+      <c r="A25" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P25" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" ht="28.8" spans="1:16">
       <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-    </row>
-    <row r="27" ht="15" spans="1:16">
+      <c r="B26" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P26" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" ht="28.8" spans="1:16">
       <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-    </row>
-    <row r="28" ht="15" spans="1:16">
+      <c r="B27" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N27" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P27" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" ht="28.8" spans="1:16">
       <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-    </row>
-    <row r="29" ht="15" spans="1:16">
+      <c r="B28" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O28" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P28" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="14"/>
@@ -5417,7 +5931,7 @@
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
     </row>
-    <row r="30" ht="15" spans="1:16">
+    <row r="30" spans="1:16">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="14"/>
@@ -5435,7 +5949,7 @@
       <c r="O30" s="14"/>
       <c r="P30" s="14"/>
     </row>
-    <row r="31" ht="15" spans="1:16">
+    <row r="31" spans="1:16">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="14"/>
@@ -5453,7 +5967,7 @@
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
     </row>
-    <row r="32" ht="15" spans="1:16">
+    <row r="32" spans="1:16">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="14"/>
@@ -5471,7 +5985,7 @@
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
     </row>
-    <row r="33" ht="15" spans="1:16">
+    <row r="33" spans="1:16">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="14"/>
@@ -6083,59 +6597,17 @@
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
     </row>
-    <row r="67" ht="15" spans="1:16">
-      <c r="A67" s="14"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
+    <row r="67" spans="12:13">
       <c r="L67" s="14"/>
       <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="14"/>
-      <c r="P67" s="14"/>
-    </row>
-    <row r="68" ht="15" spans="1:16">
-      <c r="A68" s="14"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
+    </row>
+    <row r="68" spans="12:13">
       <c r="L68" s="14"/>
       <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="14"/>
-      <c r="P68" s="14"/>
-    </row>
-    <row r="69" ht="15" spans="1:16">
-      <c r="A69" s="14"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
+    </row>
+    <row r="69" spans="12:13">
       <c r="L69" s="14"/>
       <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
-      <c r="O69" s="14"/>
-      <c r="P69" s="14"/>
     </row>
     <row r="70" spans="12:13">
       <c r="L70" s="14"/>
@@ -55417,25 +55889,13 @@
       <c r="L12389" s="14"/>
       <c r="M12389" s="14"/>
     </row>
-    <row r="12390" spans="12:13">
-      <c r="L12390" s="14"/>
-      <c r="M12390" s="14"/>
-    </row>
-    <row r="12391" spans="12:13">
-      <c r="L12391" s="14"/>
-      <c r="M12391" s="14"/>
-    </row>
-    <row r="12392" spans="12:13">
-      <c r="L12392" s="14"/>
-      <c r="M12392" s="14"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 L13 M15 M16 L17 M17 L18 M18 L5:L6 L7:L8 L9:L10 L11:L12 L14:L16 M4:M6 M7:M8 M9:M14 L19:M12392">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 M2 L3 M3 L4 L13 M15 M16 M17 L20 L25:M25 L5:L6 L7:L8 L9:L10 L11:L12 L14:L16 L17:L19 L21:L24 L26:L28 M4:M6 M7:M8 M9:M14 M18:M19 M20:M24 M26:M28 L29:M12389">
       <formula1>Result</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12393:M65539">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12390:M65536">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -55463,7 +55923,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -55473,7 +55933,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -55482,7 +55942,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -55491,7 +55951,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -55500,7 +55960,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -55509,7 +55969,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -55518,7 +55978,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -55527,7 +55987,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -55536,7 +55996,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -55545,7 +56005,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>